<commit_message>
Mise à jour du tableau de répartition des audiences (1.09.2025)
10 corrections appliquées:
- 9h 12 JU: VEN sem 3 (MP→E), VEN sem 5 (MP→A)
- 9h 18 JU: MAR sem 3 (MP→A), MAR sem 4 (MP→S)
- 9h 20 JU: MAR sem 4 (A→MP)
- 9h CRPC: JEU sem 3 (S→MP)
- 13h30 16-CI: VEN sem 4 (MP→V/C)
- 13h30 20 Coll: LUN sem 3 (M→MP), LUN sem 5 (MP→M), MER sem 1 (MP→M)

https://claude.ai/code/session_013GVFUnsuJT5neVS5zgeUHQ
</commit_message>
<xml_diff>
--- a/data/tableau_repartition_audiences.xlsx
+++ b/data/tableau_repartition_audiences.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MagPlan\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marion.chalaux\Documents\SG NTR\Organisation Parquet\Tableau répartition audiences\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32021317-D5BE-4E81-89A5-07213F1F0093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6008F25-1D3B-49E9-BC35-2EC725D85A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <sheet name="Feuil3" sheetId="6" state="hidden" r:id="rId7"/>
     <sheet name="Charges" sheetId="2" state="hidden" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="325">
   <si>
     <t>LUNDI</t>
   </si>
@@ -1145,6 +1145,9 @@
   </si>
   <si>
     <t>2 aud. 17ème Coll Presse + 2 coll</t>
+  </si>
+  <si>
+    <t>V/C</t>
   </si>
 </sst>
 </file>
@@ -2458,7 +2461,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="550">
+  <cellXfs count="548">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -3389,10 +3392,7 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3421,6 +3421,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
@@ -3430,13 +3431,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF00FF"/>
       <color rgb="FFCCFFFF"/>
       <color rgb="FFFFFFCC"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FFFF9999"/>
       <color rgb="FF009999"/>
       <color rgb="FF00FF00"/>
-      <color rgb="FFFF00FF"/>
       <color rgb="FF00FFFF"/>
       <color rgb="FF9900FF"/>
       <color rgb="FF9966FF"/>
@@ -7929,7 +7930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AR52"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="65" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B16" zoomScale="65" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -14142,32 +14143,8 @@
       <c r="AO70" s="292"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AF10:AG10">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF30:AG30">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH10:AI10 AK10:AL10 AN10:AQ10">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="AH30:AQ30">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14178,8 +14155,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH30:AQ30">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="AH10:AI10 AK10:AL10 AN10:AQ10">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -14214,6 +14191,30 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AF10:AG10">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF30:AG30">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="55" orientation="landscape" r:id="rId1"/>
 </worksheet>
@@ -14221,10 +14222,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F41151A-808E-40FA-95B0-4CC2D2969B4F}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AS53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q50" sqref="Q50"/>
+      <selection activeCell="AQ42" sqref="AQ42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14456,22 +14460,22 @@
       <c r="AI4" s="418" t="s">
         <v>45</v>
       </c>
-      <c r="AJ4" s="544" t="s">
+      <c r="AJ4" s="541" t="s">
         <v>272</v>
       </c>
-      <c r="AK4" s="543" t="s">
+      <c r="AK4" s="540" t="s">
         <v>312</v>
       </c>
       <c r="AL4" s="419" t="s">
         <v>44</v>
       </c>
-      <c r="AM4" s="541" t="s">
+      <c r="AM4" s="538" t="s">
         <v>322</v>
       </c>
       <c r="AN4" s="420" t="s">
         <v>97</v>
       </c>
-      <c r="AO4" s="542" t="s">
+      <c r="AO4" s="539" t="s">
         <v>313</v>
       </c>
       <c r="AP4" s="421" t="s">
@@ -14600,14 +14604,14 @@
         <v>49</v>
       </c>
       <c r="X6" s="392"/>
-      <c r="Y6" s="534" t="s">
-        <v>311</v>
+      <c r="Y6" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="Z6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AA6" s="535" t="s">
-        <v>311</v>
+      <c r="AA6" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="AB6" s="287">
         <v>1</v>
@@ -14634,7 +14638,7 @@
         <v>1</v>
       </c>
       <c r="AK6" s="447">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AL6" s="433">
         <v>6</v>
@@ -14679,11 +14683,11 @@
       <c r="I7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="534" t="s">
-        <v>311</v>
-      </c>
-      <c r="K7" s="534" t="s">
-        <v>311</v>
+      <c r="J7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="400" t="s">
+        <v>33</v>
       </c>
       <c r="L7" s="200" t="s">
         <v>48</v>
@@ -14731,7 +14735,7 @@
       </c>
       <c r="AE7" s="515">
         <f>SUM(AF7:AS7)</f>
-        <v>209</v>
+        <v>206.5</v>
       </c>
       <c r="AF7" s="463">
         <f>(COUNTIF($C$4:$AA$33,$AF$5))</f>
@@ -14740,23 +14744,23 @@
       <c r="AG7" s="306"/>
       <c r="AH7" s="511">
         <f>(COUNTIF($C$4:$AA$33,$AH$5))</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AI7" s="512">
         <f>(COUNTIF($C$4:$AA$33,$AI$5))-0.5</f>
-        <v>44.5</v>
+        <v>45.5</v>
       </c>
       <c r="AJ7" s="513">
-        <f>(COUNTIF($C$4:$AA$33,$AJ$5))</f>
-        <v>3</v>
+        <f>(COUNTIF($C$4:$AA$33,$AJ$5))-0.5</f>
+        <v>2.5</v>
       </c>
       <c r="AK7" s="513">
-        <f>(COUNTIF($C$4:$AA$33,$AK$5))</f>
-        <v>9</v>
+        <f>(COUNTIF($C$4:$AA$33,$AK$5))-0.5</f>
+        <v>4.5</v>
       </c>
       <c r="AL7" s="448">
         <f>(COUNTIF($C$4:$AA$33,$AL$5))</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AM7" s="448">
         <f>(COUNTIF($C$4:$AA$33,$AM$5))</f>
@@ -14779,8 +14783,8 @@
         <v>4</v>
       </c>
       <c r="AR7" s="511">
-        <f>(COUNTIF($C$4:$AA$33,$AR$5))</f>
-        <v>13</v>
+        <f>(COUNTIF($C$4:$AA$33,$AR$5))-0.5</f>
+        <v>12.5</v>
       </c>
       <c r="AS7" s="464">
         <f>(COUNTIF($C$4:$AA$33,"SG"))</f>
@@ -14799,7 +14803,7 @@
       <c r="E8" s="31"/>
       <c r="F8" s="31"/>
       <c r="G8" s="250"/>
-      <c r="H8" s="536" t="s">
+      <c r="H8" s="534" t="s">
         <v>50</v>
       </c>
       <c r="I8" s="408" t="s">
@@ -14809,7 +14813,7 @@
         <v>33</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>48</v>
+        <v>311</v>
       </c>
       <c r="L8" s="404" t="s">
         <v>33</v>
@@ -14855,7 +14859,7 @@
       <c r="AG8" s="519"/>
       <c r="AH8" s="520">
         <f>(COUNTIF($C$22:$AA$33,AH5))+(COUNTIF($C$13:$AA$13,AH5))+(COUNTIF($C$4:$AA$11,AH5))-(COUNTIF($C$5:$AA$5,#REF!))</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AI8" s="520">
         <f>(COUNTIF($C$22:$AA$33,AI5))+(COUNTIF($C$13:$AA$13,AI5))+(COUNTIF($C$4:$AA$11,AI5))-0.5</f>
@@ -14867,11 +14871,11 @@
       </c>
       <c r="AK8" s="520">
         <f t="shared" ref="AK8" si="1">(COUNTIF($C$22:$AA$33,AK5))+(COUNTIF($C$13:$AA$13,AK5))+(COUNTIF($C$4:$AA$11,AK5))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AL8" s="520">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AM8" s="520">
         <f t="shared" ref="AM8" si="2">(COUNTIF($C$22:$AA$33,AM5))+(COUNTIF($C$13:$AA$13,AM5))+(COUNTIF($C$4:$AA$11,AM5))</f>
@@ -14936,7 +14940,7 @@
       </c>
       <c r="AE9" s="517">
         <f>SUM(AF9:AS9)</f>
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AF9" s="518"/>
       <c r="AG9" s="519"/>
@@ -14946,7 +14950,7 @@
       </c>
       <c r="AI9" s="520">
         <f t="shared" ref="AI9:AS9" si="3">(COUNTIF($C$12:$AA$20,AI5))-(COUNTIF($C$13:$AA$13,AI5))</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AJ9" s="520">
         <f t="shared" si="3"/>
@@ -14954,7 +14958,7 @@
       </c>
       <c r="AK9" s="520">
         <f t="shared" ref="AK9" si="4">(COUNTIF($C$12:$AA$20,AK5))-(COUNTIF($C$13:$AA$13,AK5))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AL9" s="520">
         <f t="shared" si="3"/>
@@ -15028,7 +15032,7 @@
         <v>50</v>
       </c>
       <c r="T10" s="526" t="s">
-        <v>33</v>
+        <v>311</v>
       </c>
       <c r="U10" s="9" t="s">
         <v>48</v>
@@ -15049,7 +15053,7 @@
       </c>
       <c r="AE10" s="488">
         <f>SUM(AF10:AS10)</f>
-        <v>248.625</v>
+        <v>246.875</v>
       </c>
       <c r="AF10" s="465">
         <f>COUNTIF($C$4:$AA$4,$AF$5)*$AB$4+COUNTIF($C$5:$AA$5,$AF$5)*$AB$5+COUNTIF($C$6:$AA$6,$AF$5)*$AB$6+COUNTIF($C$7:$AA$7,$AF$5)*$AB$7+COUNTIF($C$8:$AA$8,$AF$5)*$AB$8+COUNTIF($C$9:$AA$9,$AF$5)*$AB$9+COUNTIF($C$10:$AA$10,$AF$5)*$AB$10+COUNTIF($C$11:$AA$11,$AF$5)*$AB$11+COUNTIF($C$12:$AA$12,$AF$5)*$AB$12+COUNTIF($C$13:$AA$13,$AF$5)*$AB$13+COUNTIF($C$14:$AA$14,$AF$5)*$AB$14+COUNTIF($C$15:$AA$15,$AF$5)*$AB$15+COUNTIF($C$16:$AA$16,$AF$5)*$AB$16+COUNTIF($D$17:$AA$17,$AF$5)*$AB$17+COUNTIF($C$18:$AA$18,$AF$5)*$AB$18+COUNTIF($C$19:$AA$19,$AF$5)*$AB$19+COUNTIF($C$20:$AA$20,$AF$5)*$AB$20+COUNTIF($C$21:$AA$21,$AF$5)*$AB$21+COUNTIF($C$22:$AA$22,$AF$5)*$AB$22+COUNTIF($C$23:$AA$23,$AF$5)*$AB$23+COUNTIF($C$24:$AA$24,$AF$5)*$AB$24+COUNTIF($C$25:$AA$25,$AF$5)*$AB$25+COUNTIF($C$26:$AA$26,$AF$5)*$AB$26+COUNTIF($C$27:$AA$27,$AF$5)*$AB$27+COUNTIF($C$28:$AA$28,$AF$5)*$AB$28+COUNTIF($C$29:$AA$29,$AF$5)*$AB$29+COUNTIF($C$30:$AA$30,$AF$5)*$AB$30+COUNTIF($C$31:$AA$31,$AF$5)*$AB$31+COUNTIF($C$32:$AA$32,$AF$5)*$AB$32+COUNTIF($C$33:$AA$33,$AF$5)*$AB$33</f>
@@ -15061,11 +15065,11 @@
       </c>
       <c r="AH10" s="295">
         <f>COUNTIF($C$4:$AA$4,$AH$5)*$AB$4+COUNTIF($C$5:$AA$5,$AH$5)*$AB$5+COUNTIF($C$6:$AA$6,$AH$5)*$AB$6+COUNTIF($C$7:$AA$7,$AH$5)*$AB$7+COUNTIF($H$8:$AA$8,$AH$5)*$AB$8+COUNTIF($C$9:$AA$9,$AH$5)*$AB$9+COUNTIF($C$10:$AA$10,$AH$5)*$AB$10+COUNTIF($C$11:$AA$11,$AH$5)*$AB$11+COUNTIF($C$12:$AA$12,$AH$5)*$AB$12+COUNTIF($D$13:$AA$13,$AH$5)*$AB$13+COUNTIF($C$14:$AA$14,$AH$5)*$AB$14+COUNTIF($C$15:$AA$15,$AH$5)*$AB$15+COUNTIF($C$16:$AA$16,$AH$5)*$AB$16+COUNTIF($D$17:$AA$17,$AH$5)*$AB$17+COUNTIF($D$18:$AA$18,$AH$5)*$AB$18+COUNTIF($C$19:$AA$19,$AH$5)*$AB$19+COUNTIF($C$20:$AA$20,$AH$5)*$AB$20+COUNTIF($C$21:$AA$21,$AH$5)*$AB$21+COUNTIF($C$22:$AA$22,$AH$5)*$AB$22+COUNTIF($C$23:$AA$23,$AH$5)*$AB$23+COUNTIF($C$24:$AA$24,$AH$5)*$AB$24+COUNTIF($C$25:$AA$25,$AH$5)*$AB$25+COUNTIF($C$26:$AA$26,$AH$5)*$AB$26+COUNTIF($C$27:$AA$27,$AH$5)*$AB$27+COUNTIF($C$28:$AA$28,$AH$5)*$AB$28+COUNTIF($C$29:$AA$29,$AH$5)*$AB$29+COUNTIF($C$30:$AA$30,$AH$5)*$AB$30+COUNTIF($C$31:$AA$31,$AH$5)*$AB$31+COUNTIF($C$32:$AA$32,$AH$5)*$AB$32+COUNTIF($C$33:$AA$33,$AH$5)*$AB$33</f>
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AI10" s="295">
         <f>COUNTIF($C$4:$AA$4,$AI$5)*$AB$4+COUNTIF($C$5:$AA$5,$AI$5)*$AB$5+COUNTIF($C$6:$AA$6,$AI$5)*$AB$6+COUNTIF($C$7:$AA$7,$AI$5)*$AB$7+COUNTIF($H$8:$AA$8,$AI$5)*$AB$8+COUNTIF($C$9:$AA$9,$AI$5)*$AB$9+COUNTIF($C$10:$AA$10,$AI$5)*0.5*$AB$10+COUNTIF($C$11:$AA$11,$AI$5)*$AB$11+COUNTIF($C$12:$AA$12,$AI$5)*$AB$12+COUNTIF($D$13:$AA$13,$AI$5)*$AB$13+COUNTIF($C$14:$AA$14,$AI$5)*$AB$14+COUNTIF($C$15:$AA$15,$AI$5)*$AB$15+COUNTIF($C$16:$AA$16,$AI$5)*$AB$16+COUNTIF($D$17:$AA$17,$AI$5)*$AB$17+COUNTIF($D$18:$AA$18,$AI$5)*$AB$18+COUNTIF($C$19:$AA$19,$AI$5)*$AB$19+COUNTIF($C$20:$AA$20,$AI$5)*$AB$20+COUNTIF($C$21:$AA$21,$AI$5)*$AB$21+COUNTIF($C$22:$AA$22,$AI$5)*$AB$22+COUNTIF($C$23:$AA$23,$AI$5)*$AB$23+COUNTIF($C$24:$AA$24,$AI$5)*$AB$24+COUNTIF($C$25:$AA$25,$AI$5)*$AB$25+COUNTIF($C$26:$AA$26,$AI$5)*$AB$26+COUNTIF($C$27:$AA$27,$AI$5)*$AB$27+COUNTIF($C$28:$AA$28,$AI$5)*$AB$28+COUNTIF($C$29:$AA$29,$AI$5)*$AB$29+COUNTIF($C$30:$AA$30,$AI$5)*$AB$30+COUNTIF($C$31:$AA$31,$AI$5)*$AB$31+COUNTIF($C$32:$AA$32,$AI$5)*$AB$32+COUNTIF($C$33:$AA$33,$AI$5)*$AB$33</f>
-        <v>44.25</v>
+        <v>45.75</v>
       </c>
       <c r="AJ10" s="295">
         <f>COUNTIF($C$4:$AA$4,$AJ$5)*$AB$4+COUNTIF($C$5:$AA$5,$AJ$5)*$AB$5+COUNTIF($C$6:$AA$6,$AJ$5)*$AB$6+COUNTIF($C$7:$AA$7,$AJ$5)*$AB$7+COUNTIF($H$8:$AA$8,$AJ$5)*$AB$8+COUNTIF($C$9:$AA$9,$AJ$5)*$AB$9+COUNTIF($C$10:$AA$10,$AJ$5)*0.5*$AB$10+COUNTIF($C$11:$AA$11,$AJ$5)*$AB$11+COUNTIF($C$12:$AA$12,$AJ$5)*$AB$12+COUNTIF($D$13:$AA$13,$AJ$5)*$AB$13+COUNTIF($C$14:$AA$14,$AJ$5)*$AB$14+COUNTIF($C$15:$AA$15,$AJ$5)*$AB$15+COUNTIF($C$16:$AA$16,$AJ$5)*$AB$16+COUNTIF($D$17:$AA$17,$AJ$5)*$AB$17+COUNTIF($D$18:$AA$18,$AJ$5)*$AB$18+COUNTIF($C$19:$AA$19,$AJ$5)*$AB$19+COUNTIF($C$20:$AA$20,$AJ$5)*$AB$20+COUNTIF($C$21:$AA$21,$AJ$5)*$AB$21+COUNTIF($C$22:$AA$22,$AJ$5)*$AB$22+COUNTIF($C$23:$AA$23,$AJ$5)*$AB$23+COUNTIF($C$24:$AA$24,$AJ$5)*$AB$24+COUNTIF($C$25:$AA$25,$AJ$5)*$AB$25+COUNTIF($C$26:$AA$26,$AJ$5)*$AB$26+COUNTIF($C$27:$AA$27,$AJ$5)*$AB$27+COUNTIF($C$28:$AA$28,$AJ$5)*$AB$28+COUNTIF($C$29:$AA$29,$AJ$5)*$AB$29+COUNTIF($C$30:$AA$30,$AJ$5)*$AB$30+COUNTIF($C$31:$AA$31,$AJ$5)*$AB$31+COUNTIF($C$32:$AA$32,$AJ$5)*$AB$32+COUNTIF($C$33:$AA$33,$AJ$5)*$AB$33</f>
@@ -15073,11 +15077,11 @@
       </c>
       <c r="AK10" s="295">
         <f>COUNTIF($C$4:$AA$4,$AK$5)*$AB$4+COUNTIF($C$5:$AA$5,$AK$5)*$AB$5+COUNTIF($C$6:$AA$6,$AK$5)*$AB$6+COUNTIF($C$7:$AA$7,$AK$5)*$AB$7+COUNTIF($H$8:$AA$8,$AK$5)*$AB$8+COUNTIF($C$9:$AA$9,$AK$5)*$AB$9+COUNTIF($C$10:$AA$10,$AK$5)*0.5*$AB$10+COUNTIF($C$11:$AA$11,$AK$5)*$AB$11+COUNTIF($C$12:$AA$12,$AK$5)*$AB$12+COUNTIF($C$13:$AA$13,$AK$5)*$AB$13+COUNTIF($C$14:$AA$14,$AK$5)*$AB$14+COUNTIF($C$15:$AA$15,$AK$5)*$AB$15+COUNTIF($C$16:$AA$16,$AK$5)*$AB$16+COUNTIF($C$17:$AA$17,$AK$5)*$AB$17+COUNTIF($C$18:$AA$18,$AK$5)*$AB$18+COUNTIF($C$19:$AA$19,$AK$5)*$AB$19+COUNTIF($C$20:$AA$20,$AK$5)*$AB$20+COUNTIF($C$21:$AA$21,$AK$5)*$AB$21+COUNTIF($C$22:$AA$22,$AK$5)*$AB$22+COUNTIF($C$23:$AA$23,$AK$5)*$AB$23+COUNTIF($C$24:$AA$24,$AK$5)*$AB$24+COUNTIF($C$25:$AA$25,$AK$5)*$AB$25+COUNTIF($C$26:$AA$26,$AK$5)*$AB$26+COUNTIF($C$27:$AA$27,$AK$5)*$AB$27+COUNTIF($C$28:$AA$28,$AK$5)*$AB$28+COUNTIF($C$29:$AA$29,$AK$5)*$AB$29+COUNTIF($C$30:$AA$30,$AK$5)*$AB$30+COUNTIF($C$31:$AA$31,$AK$5)*$AB$31+COUNTIF($C$32:$AA$32,$AK$5)*$AB$32+COUNTIF($C$33:$AA$33,$AK$5)*$AB$33</f>
-        <v>11.5</v>
+        <v>5.75</v>
       </c>
       <c r="AL10" s="295">
         <f>COUNTIF($C$4:$AA$4,$AL$5)*$AB$4+COUNTIF($C$5:$AA$5,$AL$5)*$AB$5+COUNTIF($C$6:$AA$6,$AL$5)*$AB$6+COUNTIF($C$7:$AA$7,$AL$5)*$AB$7+COUNTIF($H$8:$AA$8,$AL$5)*$AB$8+COUNTIF($C$9:$AA$9,$AL$5)*$AB$9+COUNTIF($C$10:$AA$10,$AL$5)*$AB$10+COUNTIF($C$11:$AA$11,$AL$5)*$AB$11+COUNTIF($C$12:$AA$12,$AL$5)*$AB$12+COUNTIF($D$13:$AA$13,$AL$5)*$AB$13+COUNTIF($C$14:$AA$14,$AL$5)*$AB$14+COUNTIF($C$15:$AA$15,$AL$5)*$AB$15+COUNTIF($C$16:$AA$16,$AL$5)*$AB$16+COUNTIF($D$17:$AA$17,$AL$5)*$AB$17+COUNTIF($D$18:$AA$18,$AL$5)*$AB$18+COUNTIF($C$19:$AA$19,$AL$5)*$AB$19+COUNTIF($C$20:$AA$20,$AL$5)*$AB$20+COUNTIF($C$21:$AA$21,$AL$5)*$AB$21+COUNTIF($C$22:$AA$22,$AL$5)*$AB$22+COUNTIF($C$23:$AA$23,$AL$5)*$AB$23+COUNTIF($C$24:$AA$24,$AL$5)*$AB$24+COUNTIF($C$25:$AA$25,$AL$5)*$AB$25+COUNTIF($C$26:$AA$26,$AL$5)*$AB$26+COUNTIF($C$27:$AA$27,$AL$5)*$AB$27+COUNTIF($C$28:$AA$28,$AL$5)*$AB$28+COUNTIF($C$29:$AA$29,$AL$5)*$AB$29+COUNTIF($C$30:$AA$30,$AL$5)*$AB$30+COUNTIF($C$31:$AA$31,$AL$5)*$AB$31+COUNTIF($C$32:$AA$32,$AL$5)*$AB$32+COUNTIF($C$33:$AA$33,$AL$5)*$AB$33</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AM10" s="295">
         <f>COUNTIF($C$4:$AA$4,$AM$5)*$AB$4+COUNTIF($C$5:$AA$5,$AM$5)*$AB$5+COUNTIF($C$6:$AA$6,$AM$5)*$AB$6+COUNTIF($C$7:$AA$7,$AM$5)*$AB$7+COUNTIF($H$8:$AA$8,$AM$5)*$AB$8+COUNTIF($C$9:$AA$9,$AM$5)*$AB$9+COUNTIF($C$10:$AA$10,$AM$5)*$AB$10+COUNTIF($C$11:$AA$11,$AM$5)*$AB$11+COUNTIF($C$12:$AA$12,$AM$5)*$AB$12+COUNTIF($D$13:$AA$13,$AM$5)*$AB$13+COUNTIF($C$14:$AA$14,$AM$5)*$AB$14+COUNTIF($C$15:$AA$15,$AM$5)*$AB$15+COUNTIF($C$16:$AA$16,$AM$5)*$AB$16+COUNTIF($D$17:$AA$17,$AM$5)*$AB$17+COUNTIF($D$18:$AA$18,$AM$5)*$AB$18+COUNTIF($C$19:$AA$19,$AM$5)*$AB$19+COUNTIF($C$20:$AA$20,$AM$5)*$AB$20+COUNTIF($C$21:$AA$21,$AM$5)*$AB$21+COUNTIF($C$22:$AA$22,$AM$5)*$AB$22+COUNTIF($C$23:$AA$23,$AM$5)*$AB$23+COUNTIF($C$24:$AA$24,$AM$5)*$AB$24+COUNTIF($C$25:$AA$25,$AM$5)*$AB$25+COUNTIF($C$26:$AA$26,$AM$5)*$AB$26+COUNTIF($C$27:$AA$27,$AM$5)*$AB$27+COUNTIF($C$28:$AA$28,$AM$5)*$AB$28+COUNTIF($C$29:$AA$29,$AM$5)*$AB$29+COUNTIF($C$30:$AA$30,$AM$5)*$AB$30+COUNTIF($C$31:$AA$31,$AM$5)*$AB$31+COUNTIF($C$32:$AA$32,$AM$5)*$AB$32+COUNTIF($C$33:$AA$33,$AM$5)*$AB$33</f>
@@ -15085,7 +15089,7 @@
       </c>
       <c r="AN10" s="295">
         <f>COUNTIF($C$4:$AA$4,$AN$5)*$AB$4+COUNTIF($C$5:$AA$5,$AN$5)*$AB$5+COUNTIF($C$6:$AA$6,$AN$5)*$AB$6+COUNTIF($C$7:$AA$7,$AN$5)*$AB$7+COUNTIF($H$8:$AA$8,$AN$5)*$AB$8+COUNTIF($C$9:$AA$9,$AN$5)*$AB$9+COUNTIF($C$10:$AA$10,$AN$5)*$AB$10+COUNTIF($C$11:$AA$11,$AN$5)*$AB$11+COUNTIF($C$12:$AA$12,$AN$5)*$AB$12+COUNTIF($D$13:$AA$13,$AN$5)*$AB$13+COUNTIF($C$14:$AA$14,$AN$5)*$AB$14+COUNTIF($C$15:$AA$15,$AN$5)*$AB$15+COUNTIF($C$16:$AA$16,$AN$5)*$AB$16+COUNTIF($D$17:$AA$17,$AN$5)*$AB$17+COUNTIF($D$18:$AA$18,$AN$5)*$AB$18+COUNTIF($C$19:$AA$19,$AN$5)*$AB$19+COUNTIF($C$20:$AA$20,$AN$5)*$AB$20+COUNTIF($C$21:$AA$21,$AN$5)*$AB$21+COUNTIF($C$22:$AA$22,$AN$5)*$AB$22+COUNTIF($C$23:$AA$23,$AN$5)*$AB$23+COUNTIF($C$24:$AA$24,$AN$5)*$AB$24+COUNTIF($C$25:$AA$25,$AN$5)*$AB$25+COUNTIF($C$26:$AA$26,$AN$5)*$AB$26+COUNTIF($C$27:$AA$27,$AN$5)*$AB$27+COUNTIF($C$28:$AA$28,$AN$5)*$AB$28+COUNTIF($C$29:$AA$29,$AN$5)*$AB$29+COUNTIF($C$30:$AA$30,$AN$5)*$AB$30+COUNTIF($C$31:$AA$31,$AN$5)*$AB$31+COUNTIF($C$32:$AA$32,$AN$5)*$AB$32+COUNTIF($C$33:$AA$33,$AN$5)*$AB$33</f>
-        <v>22</v>
+        <v>22.5</v>
       </c>
       <c r="AO10" s="295">
         <f>COUNTIF($C$4:$AA$4,$AO$5)*$AB$4+COUNTIF($C$5:$AA$5,$AO$5)*$AB$5+COUNTIF($C$6:$AA$6,$AO$5)*$AB$6+COUNTIF($C$7:$AA$7,$AO$5)*$AB$7+COUNTIF($H$8:$AA$8,$AO$5)*$AB$8+COUNTIF($C$9:$AA$9,$AO$5)*$AB$9+COUNTIF($C$10:$AA$10,$AO$5)*0.5*$AB$10+COUNTIF($C$11:$AA$11,$AO$5)*$AB$11+COUNTIF($C$12:$AA$12,$AO$5)*$AB$12+COUNTIF($D$13:$AA$13,$AO$5)*$AB$13+COUNTIF($C$14:$AA$14,$AO$5)*$AB$14+COUNTIF($C$15:$AA$15,$AO$5)*$AB$15+COUNTIF($C$16:$AA$16,$AO$5)*$AB$16+COUNTIF($D$17:$AA$17,$AO$5)*$AB$17+COUNTIF($D$18:$AA$18,$AO$5)*$AB$18+COUNTIF($C$19:$AA$19,$AO$5)*$AB$19+COUNTIF($C$20:$AA$20,$AO$5)*$AB$20+COUNTIF($C$21:$AA$21,$AO$5)*$AB$21+COUNTIF($C$22:$AA$22,$AO$5)*$AB$22+COUNTIF($C$23:$AA$23,$AO$5)*$AB$23+COUNTIF($C$24:$AA$24,$AO$5)*$AB$24+COUNTIF($C$25:$AA$25,$AO$5)*$AB$25+COUNTIF($C$26:$AA$26,$AO$5)*$AB$26+COUNTIF($C$27:$AA$27,$AO$5)*$AB$27+COUNTIF($C$28:$AA$28,$AO$5)*$AB$28+COUNTIF($C$29:$AA$29,$AO$5)*$AB$29+COUNTIF($C$30:$AA$30,$AO$5)*$AB$30+COUNTIF($C$31:$AA$31,$AO$5)*$AB$31+COUNTIF($C$32:$AA$32,$AO$5)*$AB$32+COUNTIF($C$33:$AA$33,$AO$5)*$AB$33</f>
@@ -15185,15 +15189,15 @@
       <c r="AG11" s="294"/>
       <c r="AH11" s="306">
         <f t="shared" ref="AH11:AS11" si="6">AH7/AH6</f>
-        <v>5.875</v>
+        <v>6</v>
       </c>
       <c r="AI11" s="306">
         <f t="shared" si="6"/>
-        <v>6.3571428571428568</v>
+        <v>6.5</v>
       </c>
       <c r="AJ11" s="306">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AK11" s="306">
         <f t="shared" ref="AK11" si="7">AK7/AK6</f>
@@ -15201,7 +15205,7 @@
       </c>
       <c r="AL11" s="306">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>6.166666666666667</v>
       </c>
       <c r="AM11" s="306">
         <f t="shared" ref="AM11" si="8">AM7/AM6</f>
@@ -15225,7 +15229,7 @@
       </c>
       <c r="AR11" s="306">
         <f t="shared" si="6"/>
-        <v>6.5</v>
+        <v>6.25</v>
       </c>
       <c r="AS11" s="468">
         <f t="shared" si="6"/>
@@ -15294,7 +15298,7 @@
       </c>
       <c r="AE12" s="488">
         <f>(AE10-AG10)/AE13</f>
-        <v>6.8484848484848486</v>
+        <v>6.7954545454545459</v>
       </c>
       <c r="AF12" s="465">
         <f>AF10/AF13</f>
@@ -15303,11 +15307,11 @@
       <c r="AG12" s="295"/>
       <c r="AH12" s="295">
         <f>(AH10-4)/AH6</f>
-        <v>6.125</v>
+        <v>6.25</v>
       </c>
       <c r="AI12" s="295">
         <f>(AI10)/AI6</f>
-        <v>6.3214285714285712</v>
+        <v>6.5357142857142856</v>
       </c>
       <c r="AJ12" s="295">
         <f>(AJ10)/AJ6</f>
@@ -15319,7 +15323,7 @@
       </c>
       <c r="AL12" s="295">
         <f>(AL10-4)/AL6</f>
-        <v>6.166666666666667</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="AM12" s="295">
         <f>(AM10)/AM6</f>
@@ -15327,7 +15331,7 @@
       </c>
       <c r="AN12" s="295">
         <f>(AN10-3)/AN6</f>
-        <v>4.75</v>
+        <v>4.875</v>
       </c>
       <c r="AO12" s="295">
         <f>(AO10)/AO6</f>
@@ -15516,7 +15520,7 @@
       </c>
       <c r="AK14" s="455">
         <f t="shared" ref="AK14" si="10">AK6*25</f>
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="AL14" s="455">
         <f t="shared" si="9"/>
@@ -15734,7 +15738,7 @@
       <c r="B17" s="206" t="s">
         <v>228</v>
       </c>
-      <c r="C17" s="537" t="s">
+      <c r="C17" s="19" t="s">
         <v>311</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -15752,7 +15756,7 @@
       <c r="H17" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="I17" s="534" t="s">
+      <c r="I17" s="68" t="s">
         <v>311</v>
       </c>
       <c r="J17" s="68" t="s">
@@ -15803,8 +15807,8 @@
       <c r="Y17" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="Z17" s="534" t="s">
-        <v>311</v>
+      <c r="Z17" s="532" t="s">
+        <v>324</v>
       </c>
       <c r="AA17" s="387" t="s">
         <v>48</v>
@@ -15817,23 +15821,23 @@
       </c>
       <c r="AE17" s="492">
         <f>AE14-AE10-AE15</f>
-        <v>176.375</v>
+        <v>178.125</v>
       </c>
       <c r="AF17" s="476"/>
       <c r="AG17" s="305"/>
       <c r="AH17" s="305">
         <f>AH14-AH10-AH15</f>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AI17" s="305">
         <f>AI14-AI10-AI15</f>
-        <v>30.75</v>
+        <v>29.25</v>
       </c>
       <c r="AJ17" s="305"/>
       <c r="AK17" s="305"/>
       <c r="AL17" s="305">
         <f>AL14-AL10-AL15</f>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM17" s="305">
         <f>AM14-AM10-AM15</f>
@@ -15841,7 +15845,7 @@
       </c>
       <c r="AN17" s="305">
         <f>AN14-AN10-AN15</f>
-        <v>28</v>
+        <v>27.5</v>
       </c>
       <c r="AO17" s="305"/>
       <c r="AP17" s="305">
@@ -15873,11 +15877,11 @@
       <c r="E18" s="282"/>
       <c r="F18" s="282"/>
       <c r="G18" s="284"/>
-      <c r="H18" s="538" t="s">
+      <c r="H18" s="535" t="s">
         <v>274</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="539" t="s">
+      <c r="J18" s="536" t="s">
         <v>274</v>
       </c>
       <c r="K18" s="2"/>
@@ -15894,7 +15898,6 @@
       <c r="V18" s="7"/>
       <c r="W18" s="6"/>
       <c r="X18" s="58"/>
-      <c r="Z18" s="2"/>
       <c r="AA18" s="7"/>
       <c r="AB18" s="287">
         <v>1</v>
@@ -15904,23 +15907,23 @@
       </c>
       <c r="AE18" s="493">
         <f>AE17/33</f>
-        <v>5.3446969696969697</v>
+        <v>5.3977272727272725</v>
       </c>
       <c r="AF18" s="478"/>
       <c r="AG18" s="301"/>
       <c r="AH18" s="329">
         <f>AH17/AH6</f>
-        <v>5.875</v>
+        <v>5.75</v>
       </c>
       <c r="AI18" s="329">
         <f>AI17/AI6</f>
-        <v>4.3928571428571432</v>
+        <v>4.1785714285714288</v>
       </c>
       <c r="AJ18" s="329"/>
       <c r="AK18" s="329"/>
       <c r="AL18" s="329">
         <f>AL17/AL6</f>
-        <v>9.8333333333333339</v>
+        <v>9.6666666666666661</v>
       </c>
       <c r="AM18" s="329">
         <f>AM17/AM6</f>
@@ -15928,7 +15931,7 @@
       </c>
       <c r="AN18" s="329">
         <f>AN17/AN6</f>
-        <v>7</v>
+        <v>6.875</v>
       </c>
       <c r="AO18" s="329"/>
       <c r="AP18" s="329">
@@ -16012,23 +16015,23 @@
       </c>
       <c r="AE19" s="494">
         <f>AE18/2</f>
-        <v>2.6723484848484849</v>
+        <v>2.6988636363636362</v>
       </c>
       <c r="AF19" s="480"/>
       <c r="AG19" s="481"/>
       <c r="AH19" s="482">
         <f>AH18/2</f>
-        <v>2.9375</v>
+        <v>2.875</v>
       </c>
       <c r="AI19" s="482">
         <f>AI18/2</f>
-        <v>2.1964285714285716</v>
+        <v>2.0892857142857144</v>
       </c>
       <c r="AJ19" s="482"/>
       <c r="AK19" s="482"/>
       <c r="AL19" s="482">
         <f>AL18/2</f>
-        <v>4.916666666666667</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="AM19" s="482">
         <f>AM18/2</f>
@@ -16036,7 +16039,7 @@
       </c>
       <c r="AN19" s="482">
         <f>AN18/2</f>
-        <v>3.5</v>
+        <v>3.4375</v>
       </c>
       <c r="AO19" s="482"/>
       <c r="AP19" s="482">
@@ -16064,21 +16067,21 @@
         <v>50</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>50</v>
+        <v>311</v>
       </c>
       <c r="F20" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="535" t="s">
-        <v>311</v>
+      <c r="G20" s="252" t="s">
+        <v>50</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="7"/>
-      <c r="M20" s="537" t="s">
-        <v>311</v>
+      <c r="M20" s="547" t="s">
+        <v>50</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="23" t="s">
@@ -16141,7 +16144,7 @@
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="545" t="s">
+      <c r="E22" s="542" t="s">
         <v>321</v>
       </c>
       <c r="F22" s="2"/>
@@ -16386,12 +16389,12 @@
       <c r="AD26" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="AE26" s="546"/>
-      <c r="AF26" s="547"/>
-      <c r="AG26" s="547"/>
-      <c r="AH26" s="547"/>
-      <c r="AI26" s="547"/>
-      <c r="AJ26" s="548"/>
+      <c r="AE26" s="543"/>
+      <c r="AF26" s="544"/>
+      <c r="AG26" s="544"/>
+      <c r="AH26" s="544"/>
+      <c r="AI26" s="544"/>
+      <c r="AJ26" s="545"/>
       <c r="AK26" s="41">
         <v>0</v>
       </c>
@@ -16705,19 +16708,19 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="7"/>
-      <c r="H32" s="545" t="s">
+      <c r="H32" s="542" t="s">
         <v>321</v>
       </c>
-      <c r="I32" s="545" t="s">
+      <c r="I32" s="542" t="s">
         <v>321</v>
       </c>
-      <c r="J32" s="545" t="s">
+      <c r="J32" s="542" t="s">
         <v>321</v>
       </c>
-      <c r="K32" s="545" t="s">
+      <c r="K32" s="542" t="s">
         <v>321</v>
       </c>
-      <c r="L32" s="545" t="s">
+      <c r="L32" s="542" t="s">
         <v>321</v>
       </c>
       <c r="M32" s="14" t="s">
@@ -16852,7 +16855,7 @@
       <c r="AQ36" s="292"/>
     </row>
     <row r="37" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A37" s="539"/>
+      <c r="A37" s="536"/>
       <c r="B37" t="s">
         <v>317</v>
       </c>
@@ -17098,7 +17101,7 @@
       <c r="AC44" s="286"/>
     </row>
     <row r="45" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="B45" s="540" t="s">
+      <c r="B45" s="537" t="s">
         <v>318</v>
       </c>
       <c r="C45" s="411"/>
@@ -17340,7 +17343,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="41" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -23208,10 +23212,10 @@
         <f>(47-3.5*5)/10*2</f>
         <v>5.9</v>
       </c>
-      <c r="AT48" s="549" t="s">
+      <c r="AT48" s="546" t="s">
         <v>59</v>
       </c>
-      <c r="AU48" s="549"/>
+      <c r="AU48" s="546"/>
     </row>
     <row r="49" spans="28:48" ht="15.5" x14ac:dyDescent="0.35">
       <c r="AB49" s="143" t="s">

</xml_diff>